<commit_message>
GDE-7941: Added Verification of fields for ALERT_001
</commit_message>
<xml_diff>
--- a/DataSet/Integration_DataSet/Extracts/DNR/DNR_Dataset_AU.xlsx
+++ b/DataSet/Integration_DataSet/Extracts/DNR/DNR_Dataset_AU.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Evergreen\fms_cba\DataSet\Integration_DataSet\Extracts\DNR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FFE661E-7A9C-42FD-B1E8-C8B5E6B69D95}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7583741D-7069-442F-A410-6BC5CF435CB3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{BE8D4E12-2DF3-41AE-8555-AE2A983F86C9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{BE8D4E12-2DF3-41AE-8555-AE2A983F86C9}"/>
   </bookViews>
   <sheets>
     <sheet name="DNR" sheetId="2" r:id="rId1"/>
     <sheet name="CMMNT" sheetId="3" r:id="rId2"/>
-    <sheet name="SC2_DealSetup" sheetId="1" r:id="rId3"/>
+    <sheet name="ALERT" sheetId="4" r:id="rId3"/>
+    <sheet name="SC2_DealSetup" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="208">
   <si>
     <t>rowid</t>
   </si>
@@ -640,13 +641,25 @@
     <t>Columns_To_Validate</t>
   </si>
   <si>
-    <t>Report Name:|Date Range:|To Date:</t>
-  </si>
-  <si>
     <t>Delimiter</t>
   </si>
   <si>
     <t>|</t>
+  </si>
+  <si>
+    <t>ALERT_001</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Report Name:|Date Range:|To Date: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Report Name:|From Date:|To Date: </t>
   </si>
 </sst>
 </file>
@@ -1135,10 +1148,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F202B85-76BE-4B84-A6D1-C0DFB1728BAE}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1191,6 +1204,23 @@
         <v>194</v>
       </c>
     </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>204</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>205</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1200,8 +1230,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE79DBE8-E477-44B4-9F09-92E3B85F8781}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1225,7 +1255,7 @@
         <v>196</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E1" s="18" t="s">
         <v>198</v>
@@ -1245,13 +1275,13 @@
         <v>195</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>199</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
     </row>
   </sheetData>
@@ -1260,6 +1290,68 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EB52E21-7788-49EE-AC26-7FEEA4EB18E0}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="75.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="43" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="19" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>196</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>198</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>202</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>207</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D08E9AE5-79E7-4891-96CA-846CB86368D1}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>

</xml_diff>

<commit_message>
GDE-7942: Added Validation of fields in sequence for ALERT_002
</commit_message>
<xml_diff>
--- a/DataSet/Integration_DataSet/Extracts/DNR/DNR_Dataset_AU.xlsx
+++ b/DataSet/Integration_DataSet/Extracts/DNR/DNR_Dataset_AU.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Evergreen\fms_cba\DataSet\Integration_DataSet\Extracts\DNR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4937281C-A125-4854-BA13-48D56B7C6427}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E029F3A8-6AD7-4690-80A2-3AD81762C6EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{BE8D4E12-2DF3-41AE-8555-AE2A983F86C9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{BE8D4E12-2DF3-41AE-8555-AE2A983F86C9}"/>
   </bookViews>
   <sheets>
     <sheet name="DNR" sheetId="2" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="226">
   <si>
     <t>rowid</t>
   </si>
@@ -702,6 +702,12 @@
   </si>
   <si>
     <t>Deal Name|Deal Tracking Number|Comment Heading|Comment Detail|User ID|Date Added / Amended</t>
+  </si>
+  <si>
+    <t>ALERT_002</t>
+  </si>
+  <si>
+    <t>Deal Name|Deal Tracking Number|Alert Heading|Alert Content|User Name|Date Added / Amended</t>
   </si>
 </sst>
 </file>
@@ -1315,8 +1321,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE79DBE8-E477-44B4-9F09-92E3B85F8781}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1508,10 +1514,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D2ADF88-2E0D-46DB-834F-029AEE142C3D}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1520,7 +1526,7 @@
     <col min="3" max="3" width="75.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="43" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="85.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="19" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
@@ -1561,6 +1567,26 @@
       </c>
       <c r="F2" s="8" t="s">
         <v>212</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>224</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="D3" t="s">
+        <v>203</v>
+      </c>
+      <c r="E3" t="s">
+        <v>222</v>
+      </c>
+      <c r="F3" s="28" t="s">
+        <v>225</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
GDE-7943: Added Facility Field Validation for ALERT_003
</commit_message>
<xml_diff>
--- a/DataSet/Integration_DataSet/Extracts/DNR/DNR_Dataset_AU.xlsx
+++ b/DataSet/Integration_DataSet/Extracts/DNR/DNR_Dataset_AU.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Evergreen\fms_cba\DataSet\Integration_DataSet\Extracts\DNR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E029F3A8-6AD7-4690-80A2-3AD81762C6EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA534645-5EC3-40D1-B909-D86DAF0BD7EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{BE8D4E12-2DF3-41AE-8555-AE2A983F86C9}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="229">
   <si>
     <t>rowid</t>
   </si>
@@ -708,6 +708,15 @@
   </si>
   <si>
     <t>Deal Name|Deal Tracking Number|Alert Heading|Alert Content|User Name|Date Added / Amended</t>
+  </si>
+  <si>
+    <t>ALERT_003</t>
+  </si>
+  <si>
+    <t>Facility_3</t>
+  </si>
+  <si>
+    <t>Deal Name|Deal Tracking Number|Facility Name|Facility FCN|Alert Heading|Alert Content|User Name|Date Added / Amended</t>
   </si>
 </sst>
 </file>
@@ -1514,10 +1523,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D2ADF88-2E0D-46DB-834F-029AEE142C3D}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1587,6 +1596,26 @@
       </c>
       <c r="F3" s="28" t="s">
         <v>225</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>226</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="D4" t="s">
+        <v>203</v>
+      </c>
+      <c r="E4" t="s">
+        <v>227</v>
+      </c>
+      <c r="F4" s="28" t="s">
+        <v>228</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
GDE-7978: pulled from dev first then updated DNR_Dataset_AU.xlsx file.
</commit_message>
<xml_diff>
--- a/DataSet/Integration_DataSet/Extracts/DNR/DNR_Dataset_AU.xlsx
+++ b/DataSet/Integration_DataSet/Extracts/DNR/DNR_Dataset_AU.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Evergreen\fms_cba\DataSet\Integration_DataSet\Extracts\DNR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA534645-5EC3-40D1-B909-D86DAF0BD7EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2869F08E-7720-4744-AE7D-33E17D063C07}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{BE8D4E12-2DF3-41AE-8555-AE2A983F86C9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{BE8D4E12-2DF3-41AE-8555-AE2A983F86C9}"/>
   </bookViews>
   <sheets>
     <sheet name="DNR" sheetId="2" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="ALERT" sheetId="5" r:id="rId4"/>
     <sheet name="SC2_DealSetup" sheetId="1" r:id="rId5"/>
     <sheet name="CALND" sheetId="4" r:id="rId6"/>
+    <sheet name="FACPF" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="232">
   <si>
     <t>rowid</t>
   </si>
@@ -717,6 +718,15 @@
   </si>
   <si>
     <t>Deal Name|Deal Tracking Number|Facility Name|Facility FCN|Alert Heading|Alert Content|User Name|Date Added / Amended</t>
+  </si>
+  <si>
+    <t>FACPF_001</t>
+  </si>
+  <si>
+    <t>FacilityPerformancePage</t>
+  </si>
+  <si>
+    <t>Deal Processing Area|Total Utilization Amount|Facility Status</t>
   </si>
 </sst>
 </file>
@@ -899,7 +909,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -951,6 +961,8 @@
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1271,17 +1283,17 @@
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.33203125" style="8" customWidth="1"/>
-    <col min="3" max="3" width="75.6640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5546875" style="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.33203125" style="17" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" style="8" customWidth="1"/>
+    <col min="3" max="3" width="75.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" style="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.28515625" style="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="19" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="19" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
@@ -1301,7 +1313,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>119</v>
       </c>
@@ -1334,17 +1346,17 @@
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.33203125" style="8" customWidth="1"/>
-    <col min="3" max="3" width="75.6640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.6640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" style="17" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="85.5546875" style="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" style="8" customWidth="1"/>
+    <col min="3" max="3" width="75.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" style="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="85.5703125" style="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="19" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="19" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
@@ -1364,7 +1376,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>119</v>
       </c>
@@ -1384,7 +1396,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="28" t="s">
         <v>182</v>
       </c>
@@ -1417,17 +1429,17 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="78" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1460,7 +1472,7 @@
       <c r="R1" s="21"/>
       <c r="S1" s="21"/>
     </row>
-    <row r="2" spans="1:19" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
         <v>119</v>
       </c>
@@ -1491,7 +1503,7 @@
       <c r="R2" s="23"/>
       <c r="S2" s="26"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>182</v>
       </c>
@@ -1511,7 +1523,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
         <v>218</v>
       </c>
@@ -1525,20 +1537,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D2ADF88-2E0D-46DB-834F-029AEE142C3D}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="75.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="85.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="75.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="85.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="19" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="19" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
@@ -1558,7 +1570,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>119</v>
       </c>
@@ -1578,7 +1590,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1598,7 +1610,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1635,115 +1647,115 @@
       <selection pane="topRight" activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.109375" style="8" customWidth="1"/>
-    <col min="2" max="2" width="11.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.140625" style="8" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" style="8" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17" style="8" customWidth="1"/>
-    <col min="4" max="4" width="16.109375" style="8" customWidth="1"/>
-    <col min="5" max="5" width="36.5546875" style="8" customWidth="1"/>
-    <col min="6" max="6" width="26.44140625" style="8" customWidth="1"/>
-    <col min="7" max="7" width="21.6640625" style="8" customWidth="1"/>
-    <col min="8" max="8" width="26.5546875" style="8" customWidth="1"/>
-    <col min="9" max="9" width="14.44140625" style="8" customWidth="1"/>
-    <col min="10" max="10" width="21.88671875" style="8" customWidth="1"/>
-    <col min="11" max="12" width="16.88671875" style="8" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" style="8" customWidth="1"/>
+    <col min="5" max="5" width="36.5703125" style="8" customWidth="1"/>
+    <col min="6" max="6" width="26.42578125" style="8" customWidth="1"/>
+    <col min="7" max="7" width="21.7109375" style="8" customWidth="1"/>
+    <col min="8" max="8" width="26.5703125" style="8" customWidth="1"/>
+    <col min="9" max="9" width="14.42578125" style="8" customWidth="1"/>
+    <col min="10" max="10" width="21.85546875" style="8" customWidth="1"/>
+    <col min="11" max="12" width="16.85546875" style="8" customWidth="1"/>
     <col min="13" max="13" width="20" style="8" customWidth="1"/>
     <col min="14" max="14" width="22" style="8" customWidth="1"/>
-    <col min="15" max="15" width="17.88671875" style="8" customWidth="1"/>
-    <col min="16" max="16" width="26.88671875" style="8" customWidth="1"/>
-    <col min="17" max="17" width="23.33203125" style="8" customWidth="1"/>
-    <col min="18" max="18" width="22.88671875" style="8" customWidth="1"/>
-    <col min="19" max="19" width="36.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="21.44140625" style="8" customWidth="1"/>
-    <col min="21" max="21" width="20.5546875" style="8" customWidth="1"/>
-    <col min="22" max="22" width="31.6640625" style="8" customWidth="1"/>
-    <col min="23" max="23" width="26.5546875" style="8" customWidth="1"/>
-    <col min="24" max="24" width="27.88671875" style="8" customWidth="1"/>
-    <col min="25" max="25" width="32.44140625" style="8" customWidth="1"/>
-    <col min="26" max="27" width="29.6640625" style="8" customWidth="1"/>
-    <col min="28" max="28" width="18.5546875" style="8" customWidth="1"/>
-    <col min="29" max="29" width="18.88671875" style="8" customWidth="1"/>
-    <col min="30" max="30" width="16.33203125" style="8" customWidth="1"/>
+    <col min="15" max="15" width="17.85546875" style="8" customWidth="1"/>
+    <col min="16" max="16" width="26.85546875" style="8" customWidth="1"/>
+    <col min="17" max="17" width="23.28515625" style="8" customWidth="1"/>
+    <col min="18" max="18" width="22.85546875" style="8" customWidth="1"/>
+    <col min="19" max="19" width="36.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="21.42578125" style="8" customWidth="1"/>
+    <col min="21" max="21" width="20.5703125" style="8" customWidth="1"/>
+    <col min="22" max="22" width="31.7109375" style="8" customWidth="1"/>
+    <col min="23" max="23" width="26.5703125" style="8" customWidth="1"/>
+    <col min="24" max="24" width="27.85546875" style="8" customWidth="1"/>
+    <col min="25" max="25" width="32.42578125" style="8" customWidth="1"/>
+    <col min="26" max="27" width="29.7109375" style="8" customWidth="1"/>
+    <col min="28" max="28" width="18.5703125" style="8" customWidth="1"/>
+    <col min="29" max="29" width="18.85546875" style="8" customWidth="1"/>
+    <col min="30" max="30" width="16.28515625" style="8" customWidth="1"/>
     <col min="31" max="31" width="23" style="8" customWidth="1"/>
-    <col min="32" max="32" width="20.44140625" style="8" customWidth="1"/>
-    <col min="33" max="33" width="27.109375" style="8" customWidth="1"/>
-    <col min="34" max="34" width="21.109375" style="8" customWidth="1"/>
-    <col min="35" max="35" width="19.33203125" style="8" customWidth="1"/>
-    <col min="36" max="36" width="23.44140625" style="8" customWidth="1"/>
-    <col min="37" max="37" width="44.88671875" style="8" customWidth="1"/>
-    <col min="38" max="40" width="19.88671875" style="8" customWidth="1"/>
+    <col min="32" max="32" width="20.42578125" style="8" customWidth="1"/>
+    <col min="33" max="33" width="27.140625" style="8" customWidth="1"/>
+    <col min="34" max="34" width="21.140625" style="8" customWidth="1"/>
+    <col min="35" max="35" width="19.28515625" style="8" customWidth="1"/>
+    <col min="36" max="36" width="23.42578125" style="8" customWidth="1"/>
+    <col min="37" max="37" width="44.85546875" style="8" customWidth="1"/>
+    <col min="38" max="40" width="19.85546875" style="8" customWidth="1"/>
     <col min="41" max="41" width="25" style="8" customWidth="1"/>
-    <col min="42" max="42" width="24.44140625" style="8" customWidth="1"/>
-    <col min="43" max="43" width="28.88671875" style="8" customWidth="1"/>
+    <col min="42" max="42" width="24.42578125" style="8" customWidth="1"/>
+    <col min="43" max="43" width="28.85546875" style="8" customWidth="1"/>
     <col min="44" max="44" width="36" style="8" customWidth="1"/>
-    <col min="45" max="45" width="34.44140625" style="8" customWidth="1"/>
-    <col min="46" max="46" width="26.6640625" style="8" customWidth="1"/>
-    <col min="47" max="47" width="17.33203125" style="8" customWidth="1"/>
-    <col min="48" max="48" width="27.109375" style="8" customWidth="1"/>
-    <col min="49" max="49" width="35.109375" style="8" customWidth="1"/>
-    <col min="50" max="50" width="29.44140625" style="8" customWidth="1"/>
-    <col min="51" max="52" width="25.88671875" style="8" customWidth="1"/>
-    <col min="53" max="53" width="34.88671875" style="8" customWidth="1"/>
-    <col min="54" max="54" width="18.109375" style="8" customWidth="1"/>
+    <col min="45" max="45" width="34.42578125" style="8" customWidth="1"/>
+    <col min="46" max="46" width="26.7109375" style="8" customWidth="1"/>
+    <col min="47" max="47" width="17.28515625" style="8" customWidth="1"/>
+    <col min="48" max="48" width="27.140625" style="8" customWidth="1"/>
+    <col min="49" max="49" width="35.140625" style="8" customWidth="1"/>
+    <col min="50" max="50" width="29.42578125" style="8" customWidth="1"/>
+    <col min="51" max="52" width="25.85546875" style="8" customWidth="1"/>
+    <col min="53" max="53" width="34.85546875" style="8" customWidth="1"/>
+    <col min="54" max="54" width="18.140625" style="8" customWidth="1"/>
     <col min="55" max="55" width="19" style="8" customWidth="1"/>
-    <col min="56" max="56" width="32.44140625" style="8" customWidth="1"/>
-    <col min="57" max="57" width="17.33203125" style="8" customWidth="1"/>
-    <col min="58" max="58" width="26.33203125" style="8" customWidth="1"/>
-    <col min="59" max="59" width="23.5546875" style="8" customWidth="1"/>
+    <col min="56" max="56" width="32.42578125" style="8" customWidth="1"/>
+    <col min="57" max="57" width="17.28515625" style="8" customWidth="1"/>
+    <col min="58" max="58" width="26.28515625" style="8" customWidth="1"/>
+    <col min="59" max="59" width="23.5703125" style="8" customWidth="1"/>
     <col min="60" max="60" width="28" style="8" customWidth="1"/>
-    <col min="61" max="61" width="34.88671875" style="8" customWidth="1"/>
-    <col min="62" max="63" width="21.109375" style="8" customWidth="1"/>
+    <col min="61" max="61" width="34.85546875" style="8" customWidth="1"/>
+    <col min="62" max="63" width="21.140625" style="8" customWidth="1"/>
     <col min="64" max="64" width="21" style="8" customWidth="1"/>
     <col min="65" max="66" width="22" style="8" customWidth="1"/>
-    <col min="67" max="67" width="17.6640625" style="8" customWidth="1"/>
-    <col min="68" max="68" width="24.5546875" style="8" customWidth="1"/>
-    <col min="69" max="71" width="19.44140625" style="8" customWidth="1"/>
-    <col min="72" max="72" width="21.109375" style="8" customWidth="1"/>
-    <col min="73" max="75" width="17.33203125" style="8" customWidth="1"/>
-    <col min="76" max="78" width="17.5546875" style="8" customWidth="1"/>
-    <col min="79" max="79" width="26.33203125" style="8" customWidth="1"/>
-    <col min="80" max="80" width="34.88671875" style="8" customWidth="1"/>
-    <col min="81" max="81" width="26.5546875" style="8" customWidth="1"/>
-    <col min="82" max="82" width="27.33203125" style="8" customWidth="1"/>
+    <col min="67" max="67" width="17.7109375" style="8" customWidth="1"/>
+    <col min="68" max="68" width="24.5703125" style="8" customWidth="1"/>
+    <col min="69" max="71" width="19.42578125" style="8" customWidth="1"/>
+    <col min="72" max="72" width="21.140625" style="8" customWidth="1"/>
+    <col min="73" max="75" width="17.28515625" style="8" customWidth="1"/>
+    <col min="76" max="78" width="17.5703125" style="8" customWidth="1"/>
+    <col min="79" max="79" width="26.28515625" style="8" customWidth="1"/>
+    <col min="80" max="80" width="34.85546875" style="8" customWidth="1"/>
+    <col min="81" max="81" width="26.5703125" style="8" customWidth="1"/>
+    <col min="82" max="82" width="27.28515625" style="8" customWidth="1"/>
     <col min="83" max="83" width="20" style="8" customWidth="1"/>
-    <col min="84" max="84" width="11.88671875" style="8" customWidth="1"/>
-    <col min="85" max="85" width="19.44140625" style="8" customWidth="1"/>
+    <col min="84" max="84" width="11.85546875" style="8" customWidth="1"/>
+    <col min="85" max="85" width="19.42578125" style="8" customWidth="1"/>
     <col min="86" max="86" width="19" style="8" customWidth="1"/>
-    <col min="87" max="87" width="36.6640625" style="16" customWidth="1"/>
-    <col min="88" max="88" width="18.109375" style="16" customWidth="1"/>
-    <col min="89" max="89" width="15.5546875" style="16" customWidth="1"/>
-    <col min="90" max="90" width="23.33203125" style="16" customWidth="1"/>
-    <col min="91" max="91" width="11.33203125" style="16" customWidth="1"/>
-    <col min="92" max="92" width="8.6640625" style="16" customWidth="1"/>
-    <col min="93" max="93" width="18.6640625" style="16" customWidth="1"/>
+    <col min="87" max="87" width="36.7109375" style="16" customWidth="1"/>
+    <col min="88" max="88" width="18.140625" style="16" customWidth="1"/>
+    <col min="89" max="89" width="15.5703125" style="16" customWidth="1"/>
+    <col min="90" max="90" width="23.28515625" style="16" customWidth="1"/>
+    <col min="91" max="91" width="11.28515625" style="16" customWidth="1"/>
+    <col min="92" max="92" width="8.7109375" style="16" customWidth="1"/>
+    <col min="93" max="93" width="18.7109375" style="16" customWidth="1"/>
     <col min="94" max="94" width="18" style="16" customWidth="1"/>
-    <col min="95" max="95" width="12.6640625" style="16" customWidth="1"/>
-    <col min="96" max="96" width="11.44140625" style="16" customWidth="1"/>
-    <col min="97" max="97" width="23.44140625" style="8" customWidth="1"/>
-    <col min="98" max="98" width="42.109375" style="16" customWidth="1"/>
-    <col min="99" max="99" width="47.88671875" style="16" customWidth="1"/>
+    <col min="95" max="95" width="12.7109375" style="16" customWidth="1"/>
+    <col min="96" max="96" width="11.42578125" style="16" customWidth="1"/>
+    <col min="97" max="97" width="23.42578125" style="8" customWidth="1"/>
+    <col min="98" max="98" width="42.140625" style="16" customWidth="1"/>
+    <col min="99" max="99" width="47.85546875" style="16" customWidth="1"/>
     <col min="100" max="100" width="29" style="16" customWidth="1"/>
-    <col min="101" max="101" width="28.33203125" style="16" customWidth="1"/>
-    <col min="102" max="102" width="24.5546875" style="16" customWidth="1"/>
-    <col min="103" max="103" width="8.88671875" style="16" customWidth="1"/>
+    <col min="101" max="101" width="28.28515625" style="16" customWidth="1"/>
+    <col min="102" max="102" width="24.5703125" style="16" customWidth="1"/>
+    <col min="103" max="103" width="8.85546875" style="16" customWidth="1"/>
     <col min="104" max="104" width="25" style="16" customWidth="1"/>
-    <col min="105" max="105" width="19.33203125" style="8" customWidth="1"/>
-    <col min="106" max="106" width="28.44140625" style="8" customWidth="1"/>
-    <col min="107" max="107" width="21.109375" style="8" customWidth="1"/>
+    <col min="105" max="105" width="19.28515625" style="8" customWidth="1"/>
+    <col min="106" max="106" width="28.42578125" style="8" customWidth="1"/>
+    <col min="107" max="107" width="21.140625" style="8" customWidth="1"/>
     <col min="108" max="108" width="24" style="16" bestFit="1" customWidth="1"/>
-    <col min="109" max="109" width="20.44140625" style="8" customWidth="1"/>
+    <col min="109" max="109" width="20.42578125" style="8" customWidth="1"/>
     <col min="110" max="110" width="24" style="8" customWidth="1"/>
-    <col min="111" max="112" width="18.33203125" style="8" customWidth="1"/>
+    <col min="111" max="112" width="18.28515625" style="8" customWidth="1"/>
     <col min="113" max="113" width="35" style="8" customWidth="1"/>
-    <col min="114" max="114" width="19.33203125" style="8" customWidth="1"/>
-    <col min="115" max="115" width="32.33203125" style="8" customWidth="1"/>
-    <col min="116" max="116" width="21.109375" style="8" customWidth="1"/>
-    <col min="117" max="117" width="25.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="118" max="118" width="34.88671875" bestFit="1" customWidth="1"/>
+    <col min="114" max="114" width="19.28515625" style="8" customWidth="1"/>
+    <col min="115" max="115" width="32.28515625" style="8" customWidth="1"/>
+    <col min="116" max="116" width="21.140625" style="8" customWidth="1"/>
+    <col min="117" max="117" width="25.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="118" max="118" width="34.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:119" s="3" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:119" s="3" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2102,7 +2114,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="2" spans="1:119" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:119" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>119</v>
       </c>
@@ -2464,16 +2476,16 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="78" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2496,7 +2508,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>119</v>
       </c>
@@ -2518,6 +2530,140 @@
       <c r="G2" t="s">
         <v>210</v>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F3EB20B-8614-46B2-A574-9EAAA9937BCB}">
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="20.140625" customWidth="1"/>
+    <col min="3" max="3" width="44.85546875" customWidth="1"/>
+    <col min="4" max="4" width="13" customWidth="1"/>
+    <col min="5" max="5" width="26.42578125" customWidth="1"/>
+    <col min="6" max="6" width="53.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="29" t="s">
+        <v>196</v>
+      </c>
+      <c r="D1" s="29" t="s">
+        <v>202</v>
+      </c>
+      <c r="E1" s="29" t="s">
+        <v>198</v>
+      </c>
+      <c r="F1" s="29" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="30">
+        <v>1</v>
+      </c>
+      <c r="B2" s="30" t="s">
+        <v>229</v>
+      </c>
+      <c r="C2" s="30" t="s">
+        <v>208</v>
+      </c>
+      <c r="D2" s="30" t="s">
+        <v>203</v>
+      </c>
+      <c r="E2" s="30" t="s">
+        <v>230</v>
+      </c>
+      <c r="F2" s="30" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="30"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="30"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="30"/>
+      <c r="B5" s="30"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="30"/>
+      <c r="B6" s="30"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="30"/>
+      <c r="B7" s="30"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="30"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="30"/>
+      <c r="B8" s="30"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="30"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="30"/>
+      <c r="B9" s="30"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="30"/>
+      <c r="F9" s="30"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="30"/>
+      <c r="B10" s="30"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="30"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="30"/>
+      <c r="B11" s="30"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="30"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="30"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
GDE-7944: Added Validation for ALERT_004
</commit_message>
<xml_diff>
--- a/DataSet/Integration_DataSet/Extracts/DNR/DNR_Dataset_AU.xlsx
+++ b/DataSet/Integration_DataSet/Extracts/DNR/DNR_Dataset_AU.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Evergreen\fms_cba\DataSet\Integration_DataSet\Extracts\DNR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA534645-5EC3-40D1-B909-D86DAF0BD7EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27239E1E-B7FE-40A4-BD4A-B715F0C9AF03}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{BE8D4E12-2DF3-41AE-8555-AE2A983F86C9}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="232">
   <si>
     <t>rowid</t>
   </si>
@@ -717,6 +717,15 @@
   </si>
   <si>
     <t>Deal Name|Deal Tracking Number|Facility Name|Facility FCN|Alert Heading|Alert Content|User Name|Date Added / Amended</t>
+  </si>
+  <si>
+    <t>ALERT_004</t>
+  </si>
+  <si>
+    <t>Outstanding_4</t>
+  </si>
+  <si>
+    <t>Deal Name|Deal Tracking Number|Alias Number|Alert Heading|Alert Content|User Name|Date Added / Amended</t>
   </si>
 </sst>
 </file>
@@ -1523,10 +1532,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D2ADF88-2E0D-46DB-834F-029AEE142C3D}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1616,6 +1625,26 @@
       </c>
       <c r="F4" s="28" t="s">
         <v>228</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>229</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="D5" t="s">
+        <v>203</v>
+      </c>
+      <c r="E5" t="s">
+        <v>230</v>
+      </c>
+      <c r="F5" s="28" t="s">
+        <v>231</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
GDE-7945: Added Validation for fields in ALERT_005
</commit_message>
<xml_diff>
--- a/DataSet/Integration_DataSet/Extracts/DNR/DNR_Dataset_AU.xlsx
+++ b/DataSet/Integration_DataSet/Extracts/DNR/DNR_Dataset_AU.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Evergreen\fms_cba\DataSet\Integration_DataSet\Extracts\DNR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27239E1E-B7FE-40A4-BD4A-B715F0C9AF03}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5837F44F-6FD8-40D5-8165-798810A2259E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{BE8D4E12-2DF3-41AE-8555-AE2A983F86C9}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="235">
   <si>
     <t>rowid</t>
   </si>
@@ -726,6 +726,15 @@
   </si>
   <si>
     <t>Deal Name|Deal Tracking Number|Alias Number|Alert Heading|Alert Content|User Name|Date Added / Amended</t>
+  </si>
+  <si>
+    <t>ALERT_005</t>
+  </si>
+  <si>
+    <t>Customer_5</t>
+  </si>
+  <si>
+    <t>Customer Name|CIF Number|Alert Heading|Alert Content|User Name|Date Added / Amended</t>
   </si>
 </sst>
 </file>
@@ -1532,10 +1541,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D2ADF88-2E0D-46DB-834F-029AEE142C3D}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1645,6 +1654,26 @@
       </c>
       <c r="F5" s="28" t="s">
         <v>231</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>232</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="D6" t="s">
+        <v>203</v>
+      </c>
+      <c r="E6" t="s">
+        <v>233</v>
+      </c>
+      <c r="F6" s="28" t="s">
+        <v>234</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
GDE-7978: pulled the recent file and applied my changes
</commit_message>
<xml_diff>
--- a/DataSet/Integration_DataSet/Extracts/DNR/DNR_Dataset_AU.xlsx
+++ b/DataSet/Integration_DataSet/Extracts/DNR/DNR_Dataset_AU.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Evergreen\fms_cba\DataSet\Integration_DataSet\Extracts\DNR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u723454\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2869F08E-7720-4744-AE7D-33E17D063C07}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EB7B8C7-D09B-4B7D-AF18-21EAEC4F4468}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{BE8D4E12-2DF3-41AE-8555-AE2A983F86C9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="8" xr2:uid="{BE8D4E12-2DF3-41AE-8555-AE2A983F86C9}"/>
   </bookViews>
   <sheets>
     <sheet name="DNR" sheetId="2" r:id="rId1"/>
@@ -19,7 +19,9 @@
     <sheet name="ALERT" sheetId="5" r:id="rId4"/>
     <sheet name="SC2_DealSetup" sheetId="1" r:id="rId5"/>
     <sheet name="CALND" sheetId="4" r:id="rId6"/>
-    <sheet name="FACPF" sheetId="7" r:id="rId7"/>
+    <sheet name="LQDTY" sheetId="7" r:id="rId7"/>
+    <sheet name="AHBDE" sheetId="8" r:id="rId8"/>
+    <sheet name="Sheet1" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="244">
   <si>
     <t>rowid</t>
   </si>
@@ -718,6 +720,42 @@
   </si>
   <si>
     <t>Deal Name|Deal Tracking Number|Facility Name|Facility FCN|Alert Heading|Alert Content|User Name|Date Added / Amended</t>
+  </si>
+  <si>
+    <t>ALERT_004</t>
+  </si>
+  <si>
+    <t>Outstanding_4</t>
+  </si>
+  <si>
+    <t>Deal Name|Deal Tracking Number|Alias Number|Alert Heading|Alert Content|User Name|Date Added / Amended</t>
+  </si>
+  <si>
+    <t>LQDTY_001_DetailsTab</t>
+  </si>
+  <si>
+    <t>Details</t>
+  </si>
+  <si>
+    <t>Effective Date|TRN Group Internal ID|Transaction Id|Customer ID|Customer Name|Currency|Net Cashflow|Transaction Description|Transaction Status</t>
+  </si>
+  <si>
+    <t>LQDTY_001_SummaryTab</t>
+  </si>
+  <si>
+    <t>Summary</t>
+  </si>
+  <si>
+    <t>Effective Date|New Drawdown|Increase|Total Drawdown|Payments|Interest|Total Repayment|NetFlow</t>
+  </si>
+  <si>
+    <t>AHBDE_001</t>
+  </si>
+  <si>
+    <t>Agency_DE Extract</t>
+  </si>
+  <si>
+    <t>Customer Short Name|Host Bank Share Amount|Cashflow Currency|Cashflow Direction|Processing Date|Effective Date|DDA Transaction Description|Cashflow Description|Deal Tracking Number|Transaction Code|Expense Code|Cashflow ID|Processing Area Code|Cashflow Status|Payment Method|Cashflow Create Date/Time</t>
   </si>
   <si>
     <t>FACPF_001</t>
@@ -909,7 +947,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -961,7 +999,12 @@
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1535,10 +1578,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D2ADF88-2E0D-46DB-834F-029AEE142C3D}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1628,6 +1671,26 @@
       </c>
       <c r="F4" s="28" t="s">
         <v>228</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>229</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="D5" t="s">
+        <v>203</v>
+      </c>
+      <c r="E5" t="s">
+        <v>230</v>
+      </c>
+      <c r="F5" s="28" t="s">
+        <v>231</v>
       </c>
     </row>
   </sheetData>
@@ -2476,7 +2539,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2537,133 +2600,264 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F3EB20B-8614-46B2-A574-9EAAA9937BCB}">
-  <dimension ref="A1:F11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65A726E3-6A41-47BC-8177-FCAE7FD066CF}">
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="20.140625" customWidth="1"/>
-    <col min="3" max="3" width="44.85546875" customWidth="1"/>
-    <col min="4" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="26.42578125" customWidth="1"/>
-    <col min="6" max="6" width="53.85546875" customWidth="1"/>
+    <col min="1" max="1" width="6" style="28" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24" style="28" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="75.7109375" style="28" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" style="28" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" style="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.140625" style="17" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="19" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>196</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>202</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>198</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="29" t="s">
+        <v>119</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>232</v>
+      </c>
+      <c r="C2" s="28" t="s">
+        <v>195</v>
+      </c>
+      <c r="D2" s="28" t="s">
+        <v>203</v>
+      </c>
+      <c r="E2" s="28" t="s">
+        <v>233</v>
+      </c>
+      <c r="F2" s="28" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="29" t="s">
+        <v>182</v>
+      </c>
+      <c r="B3" s="28" t="s">
+        <v>235</v>
+      </c>
+      <c r="C3" s="28" t="s">
+        <v>195</v>
+      </c>
+      <c r="D3" s="28" t="s">
+        <v>203</v>
+      </c>
+      <c r="E3" s="28" t="s">
+        <v>236</v>
+      </c>
+      <c r="F3" s="28" t="s">
+        <v>237</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C016368-407E-42D4-B8AC-285BAED2DDB5}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="6" style="28" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24" style="28" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="75.7109375" style="28" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" style="28" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" style="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.140625" style="17" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="19" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>196</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>202</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>198</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="29" t="s">
+        <v>119</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>238</v>
+      </c>
+      <c r="C2" s="28" t="s">
+        <v>195</v>
+      </c>
+      <c r="D2" s="28" t="s">
+        <v>203</v>
+      </c>
+      <c r="E2" s="28" t="s">
+        <v>239</v>
+      </c>
+      <c r="F2" s="28" t="s">
+        <v>240</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B30C5209-2AED-4323-BD85-6CFB6EE0DA65}">
+  <dimension ref="A1:F9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.5703125" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" customWidth="1"/>
+    <col min="3" max="3" width="38.85546875" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" customWidth="1"/>
+    <col min="5" max="5" width="18.85546875" customWidth="1"/>
+    <col min="6" max="6" width="57.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="30" t="s">
         <v>196</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="D1" s="30" t="s">
         <v>202</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="E1" s="30" t="s">
         <v>198</v>
       </c>
-      <c r="F1" s="29" t="s">
+      <c r="F1" s="30" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="30">
+      <c r="A2" s="31">
         <v>1</v>
       </c>
-      <c r="B2" s="30" t="s">
-        <v>229</v>
-      </c>
-      <c r="C2" s="30" t="s">
+      <c r="B2" s="31" t="s">
+        <v>241</v>
+      </c>
+      <c r="C2" s="31" t="s">
         <v>208</v>
       </c>
-      <c r="D2" s="30" t="s">
+      <c r="D2" s="31" t="s">
         <v>203</v>
       </c>
-      <c r="E2" s="30" t="s">
-        <v>230</v>
-      </c>
-      <c r="F2" s="30" t="s">
-        <v>231</v>
+      <c r="E2" s="31" t="s">
+        <v>242</v>
+      </c>
+      <c r="F2" s="31" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="30"/>
-      <c r="B3" s="30"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
+      <c r="A3" s="31"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="30"/>
-      <c r="B4" s="30"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
+      <c r="A4" s="31"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="30"/>
-      <c r="B5" s="30"/>
-      <c r="C5" s="30"/>
-      <c r="D5" s="30"/>
-      <c r="E5" s="30"/>
-      <c r="F5" s="30"/>
+      <c r="A5" s="31"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="31"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="30"/>
-      <c r="B6" s="30"/>
-      <c r="C6" s="30"/>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="30"/>
+      <c r="A6" s="31"/>
+      <c r="B6" s="31"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="31"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="30"/>
-      <c r="B7" s="30"/>
-      <c r="C7" s="30"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="30"/>
+      <c r="A7" s="31"/>
+      <c r="B7" s="31"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="31"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="30"/>
-      <c r="B8" s="30"/>
-      <c r="C8" s="30"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="30"/>
+      <c r="A8" s="31"/>
+      <c r="B8" s="31"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="31"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="30"/>
-      <c r="B9" s="30"/>
-      <c r="C9" s="30"/>
-      <c r="D9" s="30"/>
-      <c r="E9" s="30"/>
-      <c r="F9" s="30"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="30"/>
-      <c r="B10" s="30"/>
-      <c r="C10" s="30"/>
-      <c r="D10" s="30"/>
-      <c r="E10" s="30"/>
-      <c r="F10" s="30"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="30"/>
-      <c r="B11" s="30"/>
-      <c r="C11" s="30"/>
-      <c r="D11" s="30"/>
-      <c r="E11" s="30"/>
-      <c r="F11" s="30"/>
+      <c r="A9" s="31"/>
+      <c r="B9" s="31"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="31"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
GDE-7978: pulled latest DNR_Dataset_AU.xlsx and added my dataset sheet
</commit_message>
<xml_diff>
--- a/DataSet/Integration_DataSet/Extracts/DNR/DNR_Dataset_AU.xlsx
+++ b/DataSet/Integration_DataSet/Extracts/DNR/DNR_Dataset_AU.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Evergreen\fms_cba\DataSet\Integration_DataSet\Extracts\DNR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54AA4A49-ED7B-44E3-B8A6-01631374CBCA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAD20ABE-9781-4DE2-8026-0DC1722D1491}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{BE8D4E12-2DF3-41AE-8555-AE2A983F86C9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="8" xr2:uid="{BE8D4E12-2DF3-41AE-8555-AE2A983F86C9}"/>
   </bookViews>
   <sheets>
     <sheet name="DNR" sheetId="2" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="CALND" sheetId="4" r:id="rId6"/>
     <sheet name="LQDTY" sheetId="7" r:id="rId7"/>
     <sheet name="AHBDE" sheetId="8" r:id="rId8"/>
+    <sheet name="PACPF" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="249">
   <si>
     <t>rowid</t>
   </si>
@@ -770,6 +771,15 @@
   </si>
   <si>
     <t>Deal Name|Deal Tracking Number|Alias Number|Comment Heading|Comment Detail|User ID|Date Added / Amended</t>
+  </si>
+  <si>
+    <t>FACPF_001</t>
+  </si>
+  <si>
+    <t>FacilityPerformancePage</t>
+  </si>
+  <si>
+    <t>Deal Processing Area|Total Utilization Amount|Facility Status</t>
   </si>
 </sst>
 </file>
@@ -952,7 +962,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1010,6 +1020,10 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1330,17 +1344,17 @@
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.33203125" style="8" customWidth="1"/>
-    <col min="3" max="3" width="75.6640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5546875" style="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.33203125" style="17" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" style="8" customWidth="1"/>
+    <col min="3" max="3" width="75.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" style="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.28515625" style="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="19" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="19" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
@@ -1360,7 +1374,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>119</v>
       </c>
@@ -1389,21 +1403,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE79DBE8-E477-44B4-9F09-92E3B85F8781}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.33203125" style="8" customWidth="1"/>
-    <col min="3" max="3" width="75.6640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.6640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" style="17" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="85.5546875" style="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" style="8" customWidth="1"/>
+    <col min="3" max="3" width="75.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" style="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="85.5703125" style="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="19" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="19" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
@@ -1423,7 +1437,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>119</v>
       </c>
@@ -1443,7 +1457,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="28" t="s">
         <v>182</v>
       </c>
@@ -1463,7 +1477,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A4" s="28" t="s">
         <v>218</v>
       </c>
@@ -1483,7 +1497,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="28" t="s">
         <v>243</v>
       </c>
@@ -1516,17 +1530,17 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="78" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1559,7 +1573,7 @@
       <c r="R1" s="21"/>
       <c r="S1" s="21"/>
     </row>
-    <row r="2" spans="1:19" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
         <v>119</v>
       </c>
@@ -1590,7 +1604,7 @@
       <c r="R2" s="23"/>
       <c r="S2" s="26"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>182</v>
       </c>
@@ -1610,7 +1624,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
         <v>218</v>
       </c>
@@ -1628,16 +1642,16 @@
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="75.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="85.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="75.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="85.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="19" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="19" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
@@ -1657,7 +1671,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>119</v>
       </c>
@@ -1677,7 +1691,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1697,7 +1711,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1717,7 +1731,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1754,115 +1768,115 @@
       <selection pane="topRight" activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.109375" style="8" customWidth="1"/>
-    <col min="2" max="2" width="11.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.140625" style="8" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" style="8" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17" style="8" customWidth="1"/>
-    <col min="4" max="4" width="16.109375" style="8" customWidth="1"/>
-    <col min="5" max="5" width="36.5546875" style="8" customWidth="1"/>
-    <col min="6" max="6" width="26.44140625" style="8" customWidth="1"/>
-    <col min="7" max="7" width="21.6640625" style="8" customWidth="1"/>
-    <col min="8" max="8" width="26.5546875" style="8" customWidth="1"/>
-    <col min="9" max="9" width="14.44140625" style="8" customWidth="1"/>
-    <col min="10" max="10" width="21.88671875" style="8" customWidth="1"/>
-    <col min="11" max="12" width="16.88671875" style="8" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" style="8" customWidth="1"/>
+    <col min="5" max="5" width="36.5703125" style="8" customWidth="1"/>
+    <col min="6" max="6" width="26.42578125" style="8" customWidth="1"/>
+    <col min="7" max="7" width="21.7109375" style="8" customWidth="1"/>
+    <col min="8" max="8" width="26.5703125" style="8" customWidth="1"/>
+    <col min="9" max="9" width="14.42578125" style="8" customWidth="1"/>
+    <col min="10" max="10" width="21.85546875" style="8" customWidth="1"/>
+    <col min="11" max="12" width="16.85546875" style="8" customWidth="1"/>
     <col min="13" max="13" width="20" style="8" customWidth="1"/>
     <col min="14" max="14" width="22" style="8" customWidth="1"/>
-    <col min="15" max="15" width="17.88671875" style="8" customWidth="1"/>
-    <col min="16" max="16" width="26.88671875" style="8" customWidth="1"/>
-    <col min="17" max="17" width="23.33203125" style="8" customWidth="1"/>
-    <col min="18" max="18" width="22.88671875" style="8" customWidth="1"/>
-    <col min="19" max="19" width="36.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="21.44140625" style="8" customWidth="1"/>
-    <col min="21" max="21" width="20.5546875" style="8" customWidth="1"/>
-    <col min="22" max="22" width="31.6640625" style="8" customWidth="1"/>
-    <col min="23" max="23" width="26.5546875" style="8" customWidth="1"/>
-    <col min="24" max="24" width="27.88671875" style="8" customWidth="1"/>
-    <col min="25" max="25" width="32.44140625" style="8" customWidth="1"/>
-    <col min="26" max="27" width="29.6640625" style="8" customWidth="1"/>
-    <col min="28" max="28" width="18.5546875" style="8" customWidth="1"/>
-    <col min="29" max="29" width="18.88671875" style="8" customWidth="1"/>
-    <col min="30" max="30" width="16.33203125" style="8" customWidth="1"/>
+    <col min="15" max="15" width="17.85546875" style="8" customWidth="1"/>
+    <col min="16" max="16" width="26.85546875" style="8" customWidth="1"/>
+    <col min="17" max="17" width="23.28515625" style="8" customWidth="1"/>
+    <col min="18" max="18" width="22.85546875" style="8" customWidth="1"/>
+    <col min="19" max="19" width="36.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="21.42578125" style="8" customWidth="1"/>
+    <col min="21" max="21" width="20.5703125" style="8" customWidth="1"/>
+    <col min="22" max="22" width="31.7109375" style="8" customWidth="1"/>
+    <col min="23" max="23" width="26.5703125" style="8" customWidth="1"/>
+    <col min="24" max="24" width="27.85546875" style="8" customWidth="1"/>
+    <col min="25" max="25" width="32.42578125" style="8" customWidth="1"/>
+    <col min="26" max="27" width="29.7109375" style="8" customWidth="1"/>
+    <col min="28" max="28" width="18.5703125" style="8" customWidth="1"/>
+    <col min="29" max="29" width="18.85546875" style="8" customWidth="1"/>
+    <col min="30" max="30" width="16.28515625" style="8" customWidth="1"/>
     <col min="31" max="31" width="23" style="8" customWidth="1"/>
-    <col min="32" max="32" width="20.44140625" style="8" customWidth="1"/>
-    <col min="33" max="33" width="27.109375" style="8" customWidth="1"/>
-    <col min="34" max="34" width="21.109375" style="8" customWidth="1"/>
-    <col min="35" max="35" width="19.33203125" style="8" customWidth="1"/>
-    <col min="36" max="36" width="23.44140625" style="8" customWidth="1"/>
-    <col min="37" max="37" width="44.88671875" style="8" customWidth="1"/>
-    <col min="38" max="40" width="19.88671875" style="8" customWidth="1"/>
+    <col min="32" max="32" width="20.42578125" style="8" customWidth="1"/>
+    <col min="33" max="33" width="27.140625" style="8" customWidth="1"/>
+    <col min="34" max="34" width="21.140625" style="8" customWidth="1"/>
+    <col min="35" max="35" width="19.28515625" style="8" customWidth="1"/>
+    <col min="36" max="36" width="23.42578125" style="8" customWidth="1"/>
+    <col min="37" max="37" width="44.85546875" style="8" customWidth="1"/>
+    <col min="38" max="40" width="19.85546875" style="8" customWidth="1"/>
     <col min="41" max="41" width="25" style="8" customWidth="1"/>
-    <col min="42" max="42" width="24.44140625" style="8" customWidth="1"/>
-    <col min="43" max="43" width="28.88671875" style="8" customWidth="1"/>
+    <col min="42" max="42" width="24.42578125" style="8" customWidth="1"/>
+    <col min="43" max="43" width="28.85546875" style="8" customWidth="1"/>
     <col min="44" max="44" width="36" style="8" customWidth="1"/>
-    <col min="45" max="45" width="34.44140625" style="8" customWidth="1"/>
-    <col min="46" max="46" width="26.6640625" style="8" customWidth="1"/>
-    <col min="47" max="47" width="17.33203125" style="8" customWidth="1"/>
-    <col min="48" max="48" width="27.109375" style="8" customWidth="1"/>
-    <col min="49" max="49" width="35.109375" style="8" customWidth="1"/>
-    <col min="50" max="50" width="29.44140625" style="8" customWidth="1"/>
-    <col min="51" max="52" width="25.88671875" style="8" customWidth="1"/>
-    <col min="53" max="53" width="34.88671875" style="8" customWidth="1"/>
-    <col min="54" max="54" width="18.109375" style="8" customWidth="1"/>
+    <col min="45" max="45" width="34.42578125" style="8" customWidth="1"/>
+    <col min="46" max="46" width="26.7109375" style="8" customWidth="1"/>
+    <col min="47" max="47" width="17.28515625" style="8" customWidth="1"/>
+    <col min="48" max="48" width="27.140625" style="8" customWidth="1"/>
+    <col min="49" max="49" width="35.140625" style="8" customWidth="1"/>
+    <col min="50" max="50" width="29.42578125" style="8" customWidth="1"/>
+    <col min="51" max="52" width="25.85546875" style="8" customWidth="1"/>
+    <col min="53" max="53" width="34.85546875" style="8" customWidth="1"/>
+    <col min="54" max="54" width="18.140625" style="8" customWidth="1"/>
     <col min="55" max="55" width="19" style="8" customWidth="1"/>
-    <col min="56" max="56" width="32.44140625" style="8" customWidth="1"/>
-    <col min="57" max="57" width="17.33203125" style="8" customWidth="1"/>
-    <col min="58" max="58" width="26.33203125" style="8" customWidth="1"/>
-    <col min="59" max="59" width="23.5546875" style="8" customWidth="1"/>
+    <col min="56" max="56" width="32.42578125" style="8" customWidth="1"/>
+    <col min="57" max="57" width="17.28515625" style="8" customWidth="1"/>
+    <col min="58" max="58" width="26.28515625" style="8" customWidth="1"/>
+    <col min="59" max="59" width="23.5703125" style="8" customWidth="1"/>
     <col min="60" max="60" width="28" style="8" customWidth="1"/>
-    <col min="61" max="61" width="34.88671875" style="8" customWidth="1"/>
-    <col min="62" max="63" width="21.109375" style="8" customWidth="1"/>
+    <col min="61" max="61" width="34.85546875" style="8" customWidth="1"/>
+    <col min="62" max="63" width="21.140625" style="8" customWidth="1"/>
     <col min="64" max="64" width="21" style="8" customWidth="1"/>
     <col min="65" max="66" width="22" style="8" customWidth="1"/>
-    <col min="67" max="67" width="17.6640625" style="8" customWidth="1"/>
-    <col min="68" max="68" width="24.5546875" style="8" customWidth="1"/>
-    <col min="69" max="71" width="19.44140625" style="8" customWidth="1"/>
-    <col min="72" max="72" width="21.109375" style="8" customWidth="1"/>
-    <col min="73" max="75" width="17.33203125" style="8" customWidth="1"/>
-    <col min="76" max="78" width="17.5546875" style="8" customWidth="1"/>
-    <col min="79" max="79" width="26.33203125" style="8" customWidth="1"/>
-    <col min="80" max="80" width="34.88671875" style="8" customWidth="1"/>
-    <col min="81" max="81" width="26.5546875" style="8" customWidth="1"/>
-    <col min="82" max="82" width="27.33203125" style="8" customWidth="1"/>
+    <col min="67" max="67" width="17.7109375" style="8" customWidth="1"/>
+    <col min="68" max="68" width="24.5703125" style="8" customWidth="1"/>
+    <col min="69" max="71" width="19.42578125" style="8" customWidth="1"/>
+    <col min="72" max="72" width="21.140625" style="8" customWidth="1"/>
+    <col min="73" max="75" width="17.28515625" style="8" customWidth="1"/>
+    <col min="76" max="78" width="17.5703125" style="8" customWidth="1"/>
+    <col min="79" max="79" width="26.28515625" style="8" customWidth="1"/>
+    <col min="80" max="80" width="34.85546875" style="8" customWidth="1"/>
+    <col min="81" max="81" width="26.5703125" style="8" customWidth="1"/>
+    <col min="82" max="82" width="27.28515625" style="8" customWidth="1"/>
     <col min="83" max="83" width="20" style="8" customWidth="1"/>
-    <col min="84" max="84" width="11.88671875" style="8" customWidth="1"/>
-    <col min="85" max="85" width="19.44140625" style="8" customWidth="1"/>
+    <col min="84" max="84" width="11.85546875" style="8" customWidth="1"/>
+    <col min="85" max="85" width="19.42578125" style="8" customWidth="1"/>
     <col min="86" max="86" width="19" style="8" customWidth="1"/>
-    <col min="87" max="87" width="36.6640625" style="16" customWidth="1"/>
-    <col min="88" max="88" width="18.109375" style="16" customWidth="1"/>
-    <col min="89" max="89" width="15.5546875" style="16" customWidth="1"/>
-    <col min="90" max="90" width="23.33203125" style="16" customWidth="1"/>
-    <col min="91" max="91" width="11.33203125" style="16" customWidth="1"/>
-    <col min="92" max="92" width="8.6640625" style="16" customWidth="1"/>
-    <col min="93" max="93" width="18.6640625" style="16" customWidth="1"/>
+    <col min="87" max="87" width="36.7109375" style="16" customWidth="1"/>
+    <col min="88" max="88" width="18.140625" style="16" customWidth="1"/>
+    <col min="89" max="89" width="15.5703125" style="16" customWidth="1"/>
+    <col min="90" max="90" width="23.28515625" style="16" customWidth="1"/>
+    <col min="91" max="91" width="11.28515625" style="16" customWidth="1"/>
+    <col min="92" max="92" width="8.7109375" style="16" customWidth="1"/>
+    <col min="93" max="93" width="18.7109375" style="16" customWidth="1"/>
     <col min="94" max="94" width="18" style="16" customWidth="1"/>
-    <col min="95" max="95" width="12.6640625" style="16" customWidth="1"/>
-    <col min="96" max="96" width="11.44140625" style="16" customWidth="1"/>
-    <col min="97" max="97" width="23.44140625" style="8" customWidth="1"/>
-    <col min="98" max="98" width="42.109375" style="16" customWidth="1"/>
-    <col min="99" max="99" width="47.88671875" style="16" customWidth="1"/>
+    <col min="95" max="95" width="12.7109375" style="16" customWidth="1"/>
+    <col min="96" max="96" width="11.42578125" style="16" customWidth="1"/>
+    <col min="97" max="97" width="23.42578125" style="8" customWidth="1"/>
+    <col min="98" max="98" width="42.140625" style="16" customWidth="1"/>
+    <col min="99" max="99" width="47.85546875" style="16" customWidth="1"/>
     <col min="100" max="100" width="29" style="16" customWidth="1"/>
-    <col min="101" max="101" width="28.33203125" style="16" customWidth="1"/>
-    <col min="102" max="102" width="24.5546875" style="16" customWidth="1"/>
-    <col min="103" max="103" width="8.88671875" style="16" customWidth="1"/>
+    <col min="101" max="101" width="28.28515625" style="16" customWidth="1"/>
+    <col min="102" max="102" width="24.5703125" style="16" customWidth="1"/>
+    <col min="103" max="103" width="8.85546875" style="16" customWidth="1"/>
     <col min="104" max="104" width="25" style="16" customWidth="1"/>
-    <col min="105" max="105" width="19.33203125" style="8" customWidth="1"/>
-    <col min="106" max="106" width="28.44140625" style="8" customWidth="1"/>
-    <col min="107" max="107" width="21.109375" style="8" customWidth="1"/>
+    <col min="105" max="105" width="19.28515625" style="8" customWidth="1"/>
+    <col min="106" max="106" width="28.42578125" style="8" customWidth="1"/>
+    <col min="107" max="107" width="21.140625" style="8" customWidth="1"/>
     <col min="108" max="108" width="24" style="16" bestFit="1" customWidth="1"/>
-    <col min="109" max="109" width="20.44140625" style="8" customWidth="1"/>
+    <col min="109" max="109" width="20.42578125" style="8" customWidth="1"/>
     <col min="110" max="110" width="24" style="8" customWidth="1"/>
-    <col min="111" max="112" width="18.33203125" style="8" customWidth="1"/>
+    <col min="111" max="112" width="18.28515625" style="8" customWidth="1"/>
     <col min="113" max="113" width="35" style="8" customWidth="1"/>
-    <col min="114" max="114" width="19.33203125" style="8" customWidth="1"/>
-    <col min="115" max="115" width="32.33203125" style="8" customWidth="1"/>
-    <col min="116" max="116" width="21.109375" style="8" customWidth="1"/>
-    <col min="117" max="117" width="25.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="118" max="118" width="34.88671875" bestFit="1" customWidth="1"/>
+    <col min="114" max="114" width="19.28515625" style="8" customWidth="1"/>
+    <col min="115" max="115" width="32.28515625" style="8" customWidth="1"/>
+    <col min="116" max="116" width="21.140625" style="8" customWidth="1"/>
+    <col min="117" max="117" width="25.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="118" max="118" width="34.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:119" s="3" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:119" s="3" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2221,7 +2235,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="2" spans="1:119" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:119" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>119</v>
       </c>
@@ -2586,13 +2600,13 @@
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="78" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2615,7 +2629,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>119</v>
       </c>
@@ -2651,17 +2665,17 @@
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6" style="28" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24" style="28" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="75.6640625" style="28" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.6640625" style="28" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" style="17" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="33.109375" style="17" customWidth="1"/>
+    <col min="3" max="3" width="75.7109375" style="28" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" style="28" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" style="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.140625" style="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="19" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="19" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
@@ -2681,7 +2695,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="29" t="s">
         <v>119</v>
       </c>
@@ -2701,7 +2715,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="29" t="s">
         <v>182</v>
       </c>
@@ -2734,17 +2748,17 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6" style="28" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24" style="28" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="75.6640625" style="28" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.6640625" style="28" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" style="17" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="33.109375" style="17" customWidth="1"/>
+    <col min="3" max="3" width="75.7109375" style="28" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" style="28" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" style="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.140625" style="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="19" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="19" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
@@ -2764,7 +2778,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="29" t="s">
         <v>119</v>
       </c>
@@ -2782,6 +2796,68 @@
       </c>
       <c r="F2" s="28" t="s">
         <v>240</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24AAC0C9-E4D3-47B6-B964-668D0C74A7E8}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" customWidth="1"/>
+    <col min="3" max="3" width="73.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="53" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="31" t="s">
+        <v>196</v>
+      </c>
+      <c r="D1" s="31" t="s">
+        <v>202</v>
+      </c>
+      <c r="E1" s="31" t="s">
+        <v>198</v>
+      </c>
+      <c r="F1" s="31" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="32">
+        <v>1</v>
+      </c>
+      <c r="B2" s="32" t="s">
+        <v>246</v>
+      </c>
+      <c r="C2" s="32" t="s">
+        <v>208</v>
+      </c>
+      <c r="D2" s="32" t="s">
+        <v>203</v>
+      </c>
+      <c r="E2" s="32" t="s">
+        <v>247</v>
+      </c>
+      <c r="F2" s="32" t="s">
+        <v>248</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
GDE-7978: pull recent DNR_Dataset_AU.xlsx from dev adn added my sheet
</commit_message>
<xml_diff>
--- a/DataSet/Integration_DataSet/Extracts/DNR/DNR_Dataset_AU.xlsx
+++ b/DataSet/Integration_DataSet/Extracts/DNR/DNR_Dataset_AU.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u723925\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Evergreen\fms_cba\DataSet\Integration_DataSet\Extracts\DNR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33C5A246-B270-417C-9E47-18197BBC9B8F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{081490D7-EF26-4CFD-8AC0-150F21BE329E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{BE8D4E12-2DF3-41AE-8555-AE2A983F86C9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="8" xr2:uid="{BE8D4E12-2DF3-41AE-8555-AE2A983F86C9}"/>
   </bookViews>
   <sheets>
     <sheet name="DNR" sheetId="2" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="CALND" sheetId="4" r:id="rId6"/>
     <sheet name="LQDTY" sheetId="7" r:id="rId7"/>
     <sheet name="AHBDE" sheetId="8" r:id="rId8"/>
+    <sheet name="FACPF" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="252">
   <si>
     <t>rowid</t>
   </si>
@@ -779,6 +780,15 @@
   </si>
   <si>
     <t>Customer Name|CIF Number|Alert Heading|Alert Content|User Name|Date Added / Amended</t>
+  </si>
+  <si>
+    <t>FACPF_001</t>
+  </si>
+  <si>
+    <t>FacilityPerformancePage</t>
+  </si>
+  <si>
+    <t>Deal Processing Area|Total Utilization Amount|Facility Status</t>
   </si>
 </sst>
 </file>
@@ -961,7 +971,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1019,6 +1029,10 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1339,17 +1353,17 @@
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.33203125" style="8" customWidth="1"/>
-    <col min="3" max="3" width="75.6640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5546875" style="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.33203125" style="17" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" style="8" customWidth="1"/>
+    <col min="3" max="3" width="75.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" style="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.28515625" style="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="19" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="19" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
@@ -1369,7 +1383,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>119</v>
       </c>
@@ -1402,17 +1416,17 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.33203125" style="8" customWidth="1"/>
-    <col min="3" max="3" width="75.6640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.6640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" style="17" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="85.5546875" style="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" style="8" customWidth="1"/>
+    <col min="3" max="3" width="75.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" style="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="85.5703125" style="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="19" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="19" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
@@ -1432,7 +1446,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>119</v>
       </c>
@@ -1452,7 +1466,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="28" t="s">
         <v>182</v>
       </c>
@@ -1472,7 +1486,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A4" s="28" t="s">
         <v>218</v>
       </c>
@@ -1492,7 +1506,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="28" t="s">
         <v>243</v>
       </c>
@@ -1525,17 +1539,17 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="78" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1568,7 +1582,7 @@
       <c r="R1" s="21"/>
       <c r="S1" s="21"/>
     </row>
-    <row r="2" spans="1:19" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
         <v>119</v>
       </c>
@@ -1599,7 +1613,7 @@
       <c r="R2" s="23"/>
       <c r="S2" s="26"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>182</v>
       </c>
@@ -1619,7 +1633,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
         <v>218</v>
       </c>
@@ -1633,20 +1647,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D2ADF88-2E0D-46DB-834F-029AEE142C3D}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="75.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="85.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="75.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="85.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="19" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="19" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
@@ -1666,7 +1680,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>119</v>
       </c>
@@ -1686,7 +1700,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1706,7 +1720,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1726,7 +1740,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1746,7 +1760,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1783,115 +1797,115 @@
       <selection pane="topRight" activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.109375" style="8" customWidth="1"/>
-    <col min="2" max="2" width="11.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.140625" style="8" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" style="8" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17" style="8" customWidth="1"/>
-    <col min="4" max="4" width="16.109375" style="8" customWidth="1"/>
-    <col min="5" max="5" width="36.5546875" style="8" customWidth="1"/>
-    <col min="6" max="6" width="26.44140625" style="8" customWidth="1"/>
-    <col min="7" max="7" width="21.6640625" style="8" customWidth="1"/>
-    <col min="8" max="8" width="26.5546875" style="8" customWidth="1"/>
-    <col min="9" max="9" width="14.44140625" style="8" customWidth="1"/>
-    <col min="10" max="10" width="21.88671875" style="8" customWidth="1"/>
-    <col min="11" max="12" width="16.88671875" style="8" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" style="8" customWidth="1"/>
+    <col min="5" max="5" width="36.5703125" style="8" customWidth="1"/>
+    <col min="6" max="6" width="26.42578125" style="8" customWidth="1"/>
+    <col min="7" max="7" width="21.7109375" style="8" customWidth="1"/>
+    <col min="8" max="8" width="26.5703125" style="8" customWidth="1"/>
+    <col min="9" max="9" width="14.42578125" style="8" customWidth="1"/>
+    <col min="10" max="10" width="21.85546875" style="8" customWidth="1"/>
+    <col min="11" max="12" width="16.85546875" style="8" customWidth="1"/>
     <col min="13" max="13" width="20" style="8" customWidth="1"/>
     <col min="14" max="14" width="22" style="8" customWidth="1"/>
-    <col min="15" max="15" width="17.88671875" style="8" customWidth="1"/>
-    <col min="16" max="16" width="26.88671875" style="8" customWidth="1"/>
-    <col min="17" max="17" width="23.33203125" style="8" customWidth="1"/>
-    <col min="18" max="18" width="22.88671875" style="8" customWidth="1"/>
-    <col min="19" max="19" width="36.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="21.44140625" style="8" customWidth="1"/>
-    <col min="21" max="21" width="20.5546875" style="8" customWidth="1"/>
-    <col min="22" max="22" width="31.6640625" style="8" customWidth="1"/>
-    <col min="23" max="23" width="26.5546875" style="8" customWidth="1"/>
-    <col min="24" max="24" width="27.88671875" style="8" customWidth="1"/>
-    <col min="25" max="25" width="32.44140625" style="8" customWidth="1"/>
-    <col min="26" max="27" width="29.6640625" style="8" customWidth="1"/>
-    <col min="28" max="28" width="18.5546875" style="8" customWidth="1"/>
-    <col min="29" max="29" width="18.88671875" style="8" customWidth="1"/>
-    <col min="30" max="30" width="16.33203125" style="8" customWidth="1"/>
+    <col min="15" max="15" width="17.85546875" style="8" customWidth="1"/>
+    <col min="16" max="16" width="26.85546875" style="8" customWidth="1"/>
+    <col min="17" max="17" width="23.28515625" style="8" customWidth="1"/>
+    <col min="18" max="18" width="22.85546875" style="8" customWidth="1"/>
+    <col min="19" max="19" width="36.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="21.42578125" style="8" customWidth="1"/>
+    <col min="21" max="21" width="20.5703125" style="8" customWidth="1"/>
+    <col min="22" max="22" width="31.7109375" style="8" customWidth="1"/>
+    <col min="23" max="23" width="26.5703125" style="8" customWidth="1"/>
+    <col min="24" max="24" width="27.85546875" style="8" customWidth="1"/>
+    <col min="25" max="25" width="32.42578125" style="8" customWidth="1"/>
+    <col min="26" max="27" width="29.7109375" style="8" customWidth="1"/>
+    <col min="28" max="28" width="18.5703125" style="8" customWidth="1"/>
+    <col min="29" max="29" width="18.85546875" style="8" customWidth="1"/>
+    <col min="30" max="30" width="16.28515625" style="8" customWidth="1"/>
     <col min="31" max="31" width="23" style="8" customWidth="1"/>
-    <col min="32" max="32" width="20.44140625" style="8" customWidth="1"/>
-    <col min="33" max="33" width="27.109375" style="8" customWidth="1"/>
-    <col min="34" max="34" width="21.109375" style="8" customWidth="1"/>
-    <col min="35" max="35" width="19.33203125" style="8" customWidth="1"/>
-    <col min="36" max="36" width="23.44140625" style="8" customWidth="1"/>
-    <col min="37" max="37" width="44.88671875" style="8" customWidth="1"/>
-    <col min="38" max="40" width="19.88671875" style="8" customWidth="1"/>
+    <col min="32" max="32" width="20.42578125" style="8" customWidth="1"/>
+    <col min="33" max="33" width="27.140625" style="8" customWidth="1"/>
+    <col min="34" max="34" width="21.140625" style="8" customWidth="1"/>
+    <col min="35" max="35" width="19.28515625" style="8" customWidth="1"/>
+    <col min="36" max="36" width="23.42578125" style="8" customWidth="1"/>
+    <col min="37" max="37" width="44.85546875" style="8" customWidth="1"/>
+    <col min="38" max="40" width="19.85546875" style="8" customWidth="1"/>
     <col min="41" max="41" width="25" style="8" customWidth="1"/>
-    <col min="42" max="42" width="24.44140625" style="8" customWidth="1"/>
-    <col min="43" max="43" width="28.88671875" style="8" customWidth="1"/>
+    <col min="42" max="42" width="24.42578125" style="8" customWidth="1"/>
+    <col min="43" max="43" width="28.85546875" style="8" customWidth="1"/>
     <col min="44" max="44" width="36" style="8" customWidth="1"/>
-    <col min="45" max="45" width="34.44140625" style="8" customWidth="1"/>
-    <col min="46" max="46" width="26.6640625" style="8" customWidth="1"/>
-    <col min="47" max="47" width="17.33203125" style="8" customWidth="1"/>
-    <col min="48" max="48" width="27.109375" style="8" customWidth="1"/>
-    <col min="49" max="49" width="35.109375" style="8" customWidth="1"/>
-    <col min="50" max="50" width="29.44140625" style="8" customWidth="1"/>
-    <col min="51" max="52" width="25.88671875" style="8" customWidth="1"/>
-    <col min="53" max="53" width="34.88671875" style="8" customWidth="1"/>
-    <col min="54" max="54" width="18.109375" style="8" customWidth="1"/>
+    <col min="45" max="45" width="34.42578125" style="8" customWidth="1"/>
+    <col min="46" max="46" width="26.7109375" style="8" customWidth="1"/>
+    <col min="47" max="47" width="17.28515625" style="8" customWidth="1"/>
+    <col min="48" max="48" width="27.140625" style="8" customWidth="1"/>
+    <col min="49" max="49" width="35.140625" style="8" customWidth="1"/>
+    <col min="50" max="50" width="29.42578125" style="8" customWidth="1"/>
+    <col min="51" max="52" width="25.85546875" style="8" customWidth="1"/>
+    <col min="53" max="53" width="34.85546875" style="8" customWidth="1"/>
+    <col min="54" max="54" width="18.140625" style="8" customWidth="1"/>
     <col min="55" max="55" width="19" style="8" customWidth="1"/>
-    <col min="56" max="56" width="32.44140625" style="8" customWidth="1"/>
-    <col min="57" max="57" width="17.33203125" style="8" customWidth="1"/>
-    <col min="58" max="58" width="26.33203125" style="8" customWidth="1"/>
-    <col min="59" max="59" width="23.5546875" style="8" customWidth="1"/>
+    <col min="56" max="56" width="32.42578125" style="8" customWidth="1"/>
+    <col min="57" max="57" width="17.28515625" style="8" customWidth="1"/>
+    <col min="58" max="58" width="26.28515625" style="8" customWidth="1"/>
+    <col min="59" max="59" width="23.5703125" style="8" customWidth="1"/>
     <col min="60" max="60" width="28" style="8" customWidth="1"/>
-    <col min="61" max="61" width="34.88671875" style="8" customWidth="1"/>
-    <col min="62" max="63" width="21.109375" style="8" customWidth="1"/>
+    <col min="61" max="61" width="34.85546875" style="8" customWidth="1"/>
+    <col min="62" max="63" width="21.140625" style="8" customWidth="1"/>
     <col min="64" max="64" width="21" style="8" customWidth="1"/>
     <col min="65" max="66" width="22" style="8" customWidth="1"/>
-    <col min="67" max="67" width="17.6640625" style="8" customWidth="1"/>
-    <col min="68" max="68" width="24.5546875" style="8" customWidth="1"/>
-    <col min="69" max="71" width="19.44140625" style="8" customWidth="1"/>
-    <col min="72" max="72" width="21.109375" style="8" customWidth="1"/>
-    <col min="73" max="75" width="17.33203125" style="8" customWidth="1"/>
-    <col min="76" max="78" width="17.5546875" style="8" customWidth="1"/>
-    <col min="79" max="79" width="26.33203125" style="8" customWidth="1"/>
-    <col min="80" max="80" width="34.88671875" style="8" customWidth="1"/>
-    <col min="81" max="81" width="26.5546875" style="8" customWidth="1"/>
-    <col min="82" max="82" width="27.33203125" style="8" customWidth="1"/>
+    <col min="67" max="67" width="17.7109375" style="8" customWidth="1"/>
+    <col min="68" max="68" width="24.5703125" style="8" customWidth="1"/>
+    <col min="69" max="71" width="19.42578125" style="8" customWidth="1"/>
+    <col min="72" max="72" width="21.140625" style="8" customWidth="1"/>
+    <col min="73" max="75" width="17.28515625" style="8" customWidth="1"/>
+    <col min="76" max="78" width="17.5703125" style="8" customWidth="1"/>
+    <col min="79" max="79" width="26.28515625" style="8" customWidth="1"/>
+    <col min="80" max="80" width="34.85546875" style="8" customWidth="1"/>
+    <col min="81" max="81" width="26.5703125" style="8" customWidth="1"/>
+    <col min="82" max="82" width="27.28515625" style="8" customWidth="1"/>
     <col min="83" max="83" width="20" style="8" customWidth="1"/>
-    <col min="84" max="84" width="11.88671875" style="8" customWidth="1"/>
-    <col min="85" max="85" width="19.44140625" style="8" customWidth="1"/>
+    <col min="84" max="84" width="11.85546875" style="8" customWidth="1"/>
+    <col min="85" max="85" width="19.42578125" style="8" customWidth="1"/>
     <col min="86" max="86" width="19" style="8" customWidth="1"/>
-    <col min="87" max="87" width="36.6640625" style="16" customWidth="1"/>
-    <col min="88" max="88" width="18.109375" style="16" customWidth="1"/>
-    <col min="89" max="89" width="15.5546875" style="16" customWidth="1"/>
-    <col min="90" max="90" width="23.33203125" style="16" customWidth="1"/>
-    <col min="91" max="91" width="11.33203125" style="16" customWidth="1"/>
-    <col min="92" max="92" width="8.6640625" style="16" customWidth="1"/>
-    <col min="93" max="93" width="18.6640625" style="16" customWidth="1"/>
+    <col min="87" max="87" width="36.7109375" style="16" customWidth="1"/>
+    <col min="88" max="88" width="18.140625" style="16" customWidth="1"/>
+    <col min="89" max="89" width="15.5703125" style="16" customWidth="1"/>
+    <col min="90" max="90" width="23.28515625" style="16" customWidth="1"/>
+    <col min="91" max="91" width="11.28515625" style="16" customWidth="1"/>
+    <col min="92" max="92" width="8.7109375" style="16" customWidth="1"/>
+    <col min="93" max="93" width="18.7109375" style="16" customWidth="1"/>
     <col min="94" max="94" width="18" style="16" customWidth="1"/>
-    <col min="95" max="95" width="12.6640625" style="16" customWidth="1"/>
-    <col min="96" max="96" width="11.44140625" style="16" customWidth="1"/>
-    <col min="97" max="97" width="23.44140625" style="8" customWidth="1"/>
-    <col min="98" max="98" width="42.109375" style="16" customWidth="1"/>
-    <col min="99" max="99" width="47.88671875" style="16" customWidth="1"/>
+    <col min="95" max="95" width="12.7109375" style="16" customWidth="1"/>
+    <col min="96" max="96" width="11.42578125" style="16" customWidth="1"/>
+    <col min="97" max="97" width="23.42578125" style="8" customWidth="1"/>
+    <col min="98" max="98" width="42.140625" style="16" customWidth="1"/>
+    <col min="99" max="99" width="47.85546875" style="16" customWidth="1"/>
     <col min="100" max="100" width="29" style="16" customWidth="1"/>
-    <col min="101" max="101" width="28.33203125" style="16" customWidth="1"/>
-    <col min="102" max="102" width="24.5546875" style="16" customWidth="1"/>
-    <col min="103" max="103" width="8.88671875" style="16" customWidth="1"/>
+    <col min="101" max="101" width="28.28515625" style="16" customWidth="1"/>
+    <col min="102" max="102" width="24.5703125" style="16" customWidth="1"/>
+    <col min="103" max="103" width="8.85546875" style="16" customWidth="1"/>
     <col min="104" max="104" width="25" style="16" customWidth="1"/>
-    <col min="105" max="105" width="19.33203125" style="8" customWidth="1"/>
-    <col min="106" max="106" width="28.44140625" style="8" customWidth="1"/>
-    <col min="107" max="107" width="21.109375" style="8" customWidth="1"/>
+    <col min="105" max="105" width="19.28515625" style="8" customWidth="1"/>
+    <col min="106" max="106" width="28.42578125" style="8" customWidth="1"/>
+    <col min="107" max="107" width="21.140625" style="8" customWidth="1"/>
     <col min="108" max="108" width="24" style="16" bestFit="1" customWidth="1"/>
-    <col min="109" max="109" width="20.44140625" style="8" customWidth="1"/>
+    <col min="109" max="109" width="20.42578125" style="8" customWidth="1"/>
     <col min="110" max="110" width="24" style="8" customWidth="1"/>
-    <col min="111" max="112" width="18.33203125" style="8" customWidth="1"/>
+    <col min="111" max="112" width="18.28515625" style="8" customWidth="1"/>
     <col min="113" max="113" width="35" style="8" customWidth="1"/>
-    <col min="114" max="114" width="19.33203125" style="8" customWidth="1"/>
-    <col min="115" max="115" width="32.33203125" style="8" customWidth="1"/>
-    <col min="116" max="116" width="21.109375" style="8" customWidth="1"/>
-    <col min="117" max="117" width="25.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="118" max="118" width="34.88671875" bestFit="1" customWidth="1"/>
+    <col min="114" max="114" width="19.28515625" style="8" customWidth="1"/>
+    <col min="115" max="115" width="32.28515625" style="8" customWidth="1"/>
+    <col min="116" max="116" width="21.140625" style="8" customWidth="1"/>
+    <col min="117" max="117" width="25.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="118" max="118" width="34.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:119" s="3" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:119" s="3" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2250,7 +2264,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="2" spans="1:119" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:119" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>119</v>
       </c>
@@ -2615,13 +2629,13 @@
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="78" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2644,7 +2658,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>119</v>
       </c>
@@ -2680,17 +2694,17 @@
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6" style="28" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24" style="28" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="75.6640625" style="28" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.6640625" style="28" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" style="17" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="33.109375" style="17" customWidth="1"/>
+    <col min="3" max="3" width="75.7109375" style="28" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" style="28" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" style="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.140625" style="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="19" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="19" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
@@ -2710,7 +2724,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="29" t="s">
         <v>119</v>
       </c>
@@ -2730,7 +2744,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="29" t="s">
         <v>182</v>
       </c>
@@ -2763,17 +2777,17 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6" style="28" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24" style="28" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="75.6640625" style="28" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.6640625" style="28" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" style="17" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="33.109375" style="17" customWidth="1"/>
+    <col min="3" max="3" width="75.7109375" style="28" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" style="28" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" style="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.140625" style="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="19" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="19" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
@@ -2793,7 +2807,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="29" t="s">
         <v>119</v>
       </c>
@@ -2811,6 +2825,69 @@
       </c>
       <c r="F2" s="28" t="s">
         <v>240</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B07B3A2-8FC1-4A47-B24E-FC3B5845E7C7}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="73.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="53" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="31" t="s">
+        <v>196</v>
+      </c>
+      <c r="D1" s="31" t="s">
+        <v>202</v>
+      </c>
+      <c r="E1" s="31" t="s">
+        <v>198</v>
+      </c>
+      <c r="F1" s="31" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="32">
+        <v>1</v>
+      </c>
+      <c r="B2" s="32" t="s">
+        <v>249</v>
+      </c>
+      <c r="C2" s="32" t="s">
+        <v>208</v>
+      </c>
+      <c r="D2" s="32" t="s">
+        <v>203</v>
+      </c>
+      <c r="E2" s="32" t="s">
+        <v>250</v>
+      </c>
+      <c r="F2" s="32" t="s">
+        <v>251</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
GDE-7985: added datasets, created new robot file for this test case
</commit_message>
<xml_diff>
--- a/DataSet/Integration_DataSet/Extracts/DNR/DNR_Dataset_AU.xlsx
+++ b/DataSet/Integration_DataSet/Extracts/DNR/DNR_Dataset_AU.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Evergreen\fms_cba\DataSet\Integration_DataSet\Extracts\DNR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{081490D7-EF26-4CFD-8AC0-150F21BE329E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D66BAAF-A738-4118-889B-2748A32FDC28}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="8" xr2:uid="{BE8D4E12-2DF3-41AE-8555-AE2A983F86C9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="9" xr2:uid="{BE8D4E12-2DF3-41AE-8555-AE2A983F86C9}"/>
   </bookViews>
   <sheets>
     <sheet name="DNR" sheetId="2" r:id="rId1"/>
@@ -22,6 +22,7 @@
     <sheet name="LQDTY" sheetId="7" r:id="rId7"/>
     <sheet name="AHBDE" sheetId="8" r:id="rId8"/>
     <sheet name="FACPF" sheetId="9" r:id="rId9"/>
+    <sheet name="LOACC" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="257">
   <si>
     <t>rowid</t>
   </si>
@@ -789,6 +790,21 @@
   </si>
   <si>
     <t>Deal Processing Area|Total Utilization Amount|Facility Status</t>
+  </si>
+  <si>
+    <t>Facilities</t>
+  </si>
+  <si>
+    <t>LOACC_001_FACILITIES</t>
+  </si>
+  <si>
+    <t>LOACC_001_OUTSTANDINGS</t>
+  </si>
+  <si>
+    <t>Data Type|Branch Code|Business Date|Risk Book|Portfolio|Expense Code|Deal Number|Facility Number|Facility Start Date|Facility Maturity Date|Facility Currency Code|Lender Commitment</t>
+  </si>
+  <si>
+    <t>Data Type|Outstanding Cycle Start Date|Outstanding Cycle End Date|Outstanding Cycle Due Date|Current Cycle|Outstanding Global Cycle Due|Outstanding Global Paid to Date|Outstanding Global projected EOC Accrual|Outstanding Global Projected EOC Due|Outstanding Global Accrued to Date|Branch Code|Business Date|Risk Book|Portfolio|Expense Code|Deal Number|Facility Number|Facility Start Date|Facility Maturity Date|Facility Currency Code|Lender Commitment|Outstanding Alias|Outstanding Borrower CIF|Outstanding Type|Pricing Option|Rate Basis|OST Currency Code|OST Host Bank Net|OST All-In Rate|OST Base Rate Percentage|OST Spread Percentage|OST Rate Basis|OST Effective Date|OST Repricing Frequency|OST Repricing Date</t>
   </si>
 </sst>
 </file>
@@ -879,7 +895,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -967,11 +983,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1033,6 +1058,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1408,12 +1437,95 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22B5BB90-7F29-4775-9458-F523EB169F3A}">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="118" zoomScaleNormal="118" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="73.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="188.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="31" t="s">
+        <v>196</v>
+      </c>
+      <c r="D1" s="31" t="s">
+        <v>202</v>
+      </c>
+      <c r="E1" s="31" t="s">
+        <v>198</v>
+      </c>
+      <c r="F1" s="31" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="32" t="s">
+        <v>253</v>
+      </c>
+      <c r="C2" s="32" t="s">
+        <v>208</v>
+      </c>
+      <c r="D2" s="32" t="s">
+        <v>203</v>
+      </c>
+      <c r="E2" s="32" t="s">
+        <v>252</v>
+      </c>
+      <c r="F2" s="34" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A3" s="32">
+        <v>2</v>
+      </c>
+      <c r="B3" s="32" t="s">
+        <v>254</v>
+      </c>
+      <c r="C3" s="32" t="s">
+        <v>208</v>
+      </c>
+      <c r="D3" s="32" t="s">
+        <v>203</v>
+      </c>
+      <c r="E3" s="32" t="s">
+        <v>210</v>
+      </c>
+      <c r="F3" s="33" t="s">
+        <v>256</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE79DBE8-E477-44B4-9F09-92E3B85F8781}">
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2836,8 +2948,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B07B3A2-8FC1-4A47-B24E-FC3B5845E7C7}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
GDE-7985: pulled the latest DNR_Dataset_AU.xlsx in dev and pushed to branch.
</commit_message>
<xml_diff>
--- a/DataSet/Integration_DataSet/Extracts/DNR/DNR_Dataset_AU.xlsx
+++ b/DataSet/Integration_DataSet/Extracts/DNR/DNR_Dataset_AU.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Evergreen\fms_cba\DataSet\Integration_DataSet\Extracts\DNR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D66BAAF-A738-4118-889B-2748A32FDC28}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DCDDA8A6-7401-4574-8F7D-616E226C6E9A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="9" xr2:uid="{BE8D4E12-2DF3-41AE-8555-AE2A983F86C9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="8" xr2:uid="{BE8D4E12-2DF3-41AE-8555-AE2A983F86C9}"/>
   </bookViews>
   <sheets>
     <sheet name="DNR" sheetId="2" r:id="rId1"/>
@@ -22,7 +22,6 @@
     <sheet name="LQDTY" sheetId="7" r:id="rId7"/>
     <sheet name="AHBDE" sheetId="8" r:id="rId8"/>
     <sheet name="FACPF" sheetId="9" r:id="rId9"/>
-    <sheet name="LOACC" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="258">
   <si>
     <t>rowid</t>
   </si>
@@ -783,28 +782,31 @@
     <t>Customer Name|CIF Number|Alert Heading|Alert Content|User Name|Date Added / Amended</t>
   </si>
   <si>
-    <t>FACPF_001</t>
-  </si>
-  <si>
-    <t>FacilityPerformancePage</t>
-  </si>
-  <si>
-    <t>Deal Processing Area|Total Utilization Amount|Facility Status</t>
+    <t>LOACC_001_FACILITIES</t>
   </si>
   <si>
     <t>Facilities</t>
   </si>
   <si>
-    <t>LOACC_001_FACILITIES</t>
+    <t>Data Type|Branch Code|Business Date|Risk Book|Portfolio|Expense Code|Deal Number|Facility Number|Facility Start Date|Facility Maturity Date|Facility Currency Code|Lender Commitment</t>
   </si>
   <si>
     <t>LOACC_001_OUTSTANDINGS</t>
   </si>
   <si>
-    <t>Data Type|Branch Code|Business Date|Risk Book|Portfolio|Expense Code|Deal Number|Facility Number|Facility Start Date|Facility Maturity Date|Facility Currency Code|Lender Commitment</t>
-  </si>
-  <si>
     <t>Data Type|Outstanding Cycle Start Date|Outstanding Cycle End Date|Outstanding Cycle Due Date|Current Cycle|Outstanding Global Cycle Due|Outstanding Global Paid to Date|Outstanding Global projected EOC Accrual|Outstanding Global Projected EOC Due|Outstanding Global Accrued to Date|Branch Code|Business Date|Risk Book|Portfolio|Expense Code|Deal Number|Facility Number|Facility Start Date|Facility Maturity Date|Facility Currency Code|Lender Commitment|Outstanding Alias|Outstanding Borrower CIF|Outstanding Type|Pricing Option|Rate Basis|OST Currency Code|OST Host Bank Net|OST All-In Rate|OST Base Rate Percentage|OST Spread Percentage|OST Rate Basis|OST Effective Date|OST Repricing Frequency|OST Repricing Date</t>
+  </si>
+  <si>
+    <t>LOACC_003_FACILITIES</t>
+  </si>
+  <si>
+    <t>Business Date|Facility Start Date|Facility Maturity Date</t>
+  </si>
+  <si>
+    <t>LOACC_003_OUTSTANDINGS</t>
+  </si>
+  <si>
+    <t>Business Date|Effective date of the Facility|Facility Maturity Date|Outstanding Start Date|Repricing Date|Outstanding Cycle Start Date|Outstanding Cycle End Date|Outstanding Cycle Due Date</t>
   </si>
 </sst>
 </file>
@@ -1058,10 +1060,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1437,95 +1439,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22B5BB90-7F29-4775-9458-F523EB169F3A}">
-  <dimension ref="A1:F3"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScale="118" zoomScaleNormal="118" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="73.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="188.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="31" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="31" t="s">
-        <v>196</v>
-      </c>
-      <c r="D1" s="31" t="s">
-        <v>202</v>
-      </c>
-      <c r="E1" s="31" t="s">
-        <v>198</v>
-      </c>
-      <c r="F1" s="31" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="32" t="s">
-        <v>253</v>
-      </c>
-      <c r="C2" s="32" t="s">
-        <v>208</v>
-      </c>
-      <c r="D2" s="32" t="s">
-        <v>203</v>
-      </c>
-      <c r="E2" s="32" t="s">
-        <v>252</v>
-      </c>
-      <c r="F2" s="34" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="51" x14ac:dyDescent="0.2">
-      <c r="A3" s="32">
-        <v>2</v>
-      </c>
-      <c r="B3" s="32" t="s">
-        <v>254</v>
-      </c>
-      <c r="C3" s="32" t="s">
-        <v>208</v>
-      </c>
-      <c r="D3" s="32" t="s">
-        <v>203</v>
-      </c>
-      <c r="E3" s="32" t="s">
-        <v>210</v>
-      </c>
-      <c r="F3" s="33" t="s">
-        <v>256</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE79DBE8-E477-44B4-9F09-92E3B85F8781}">
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2946,10 +2865,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B07B3A2-8FC1-4A47-B24E-FC3B5845E7C7}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2959,7 +2878,7 @@
     <col min="3" max="3" width="73.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="53" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="161.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -2983,7 +2902,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="32">
+      <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="32" t="s">
@@ -2998,8 +2917,68 @@
       <c r="E2" s="32" t="s">
         <v>250</v>
       </c>
-      <c r="F2" s="32" t="s">
+      <c r="F2" s="33" t="s">
         <v>251</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A3" s="32">
+        <v>2</v>
+      </c>
+      <c r="B3" s="32" t="s">
+        <v>252</v>
+      </c>
+      <c r="C3" s="32" t="s">
+        <v>208</v>
+      </c>
+      <c r="D3" s="32" t="s">
+        <v>203</v>
+      </c>
+      <c r="E3" s="32" t="s">
+        <v>210</v>
+      </c>
+      <c r="F3" s="34" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="32" t="s">
+        <v>254</v>
+      </c>
+      <c r="C4" s="32" t="s">
+        <v>208</v>
+      </c>
+      <c r="D4" s="32" t="s">
+        <v>203</v>
+      </c>
+      <c r="E4" s="32" t="s">
+        <v>250</v>
+      </c>
+      <c r="F4" s="32" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="32">
+        <v>4</v>
+      </c>
+      <c r="B5" s="32" t="s">
+        <v>256</v>
+      </c>
+      <c r="C5" s="32" t="s">
+        <v>208</v>
+      </c>
+      <c r="D5" s="32" t="s">
+        <v>203</v>
+      </c>
+      <c r="E5" s="32" t="s">
+        <v>210</v>
+      </c>
+      <c r="F5" s="32" t="s">
+        <v>257</v>
       </c>
     </row>
   </sheetData>

</xml_diff>